<commit_message>
new method to create grimoire
</commit_message>
<xml_diff>
--- a/data/glossar.xlsx
+++ b/data/glossar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRH\Documents\GitHub\srh_proj_dsa\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaelm\srh_proj_dsa\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DD17F8-6424-42FF-A6D0-A2F14FCF0F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB66D5-767A-4FA9-B641-02E3CF6787E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -424,13 +424,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -446,7 +446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -462,7 +462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -470,7 +470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -478,7 +478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -486,7 +486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -494,7 +494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -502,7 +502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -510,7 +510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -518,7 +518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -526,7 +526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>

</xml_diff>